<commit_message>
minor clean up + initial visualizations
</commit_message>
<xml_diff>
--- a/data_for_viewing/extracted_raw/ff_spectator_words_found_full.xlsx
+++ b/data_for_viewing/extracted_raw/ff_spectator_words_found_full.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="232">
   <si>
     <t>Filename</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>617.txt</t>
-  </si>
-  <si>
-    <t>635.txt</t>
   </si>
   <si>
     <t>Preface.txt</t>
@@ -217,8 +214,7 @@
     Mr. Thomas Inkle of London, aged twenty Years, embarked in the Downs, on the good Ship called the Achilles, bound for the West Indies, on the 16th of June 1647, in order to improve his Fortune by Trade and Merchandize. Our Adventurer was the third Son of an eminent Citizen, who had taken particular Care to instill into his Mind an early Love of Gain, by making him a perfect Master of Numbers, and consequently giving him a quick View of Loss and Advantage, and preventing the natural Impulses of his Passions, by Prepossession towards his Interests. With a Mind thus turned, young Inkle had a Person every way agreeable, a ruddy Vigour in his Countenance, Strength in his Limbs, with Ringlets of fair Hair loosely flowing on his Shoulders. It happened, in the Course of the Voyage, that the Achilles, in some Distress, put into a Creek on the Main of America, in search of Provisions. The Youth, who is the Hero of my Story, among others, went ashore on this Occasion. From their first Landing they were observed by a Party of Indians, who hid themselves in the Woods for that Purpose. The English unadvisedly marched a great distance from the Shore into the Country, and were intercepted by the Natives, who slew the greatest Number of them. Our Adventurer escaped among others, by flying into a Forest. Upon his coming into a remote and pathless Part of the Wood, he threw himself tired and breathless on a little Hillock, when an Indian Maid rushed from a Thicket behind him: After the first Surprize, they appeared mutually agreeable to each other. If the European was highly charmed with the Limbs, Features, and wild Graces of the Naked American; the American was no less taken with the Dress, Complexion, and Shape of an European, covered from Head to Foot. The Indian grew immediately enamoured of him, and consequently sollicitous for his Preservation: She therefore conveyed him to a Cave, where she gave him a Delicious Repast of Fruits, and led him to a Stream to slake his Thirst. In the midst of these good Offices, she would sometimes play with his Hair, and delight in the Opposition of its Colour to that of her Fingers: Then open his Bosome, then laugh at him for covering it. She was, it seems, a Person of Distinction, for she every day came to him in a different Dress, of the most beautiful Shells, Bugles, and Bredes. She likewise brought him a great many Spoils, which her other Lovers had presented to her; so that his Cave was richly adorned with all the spotted Skins of Beasts, and most Party-coloured Feathers of Fowls, which that World afforded. To make his Confinement more tolerable, she would carry him in the Dusk of the Evening, or by the favour of Moon-light, to unfrequented Groves, and Solitudes, and show him where to lye down in Safety, and sleep amidst the Falls of Waters, and Melody of Nightingales. Her Part was to watch and hold him in her Arms, for fear of her Country-men, and wake on Occasions to consult his Safety. In this manner did the Lovers pass away their Time, till they had learn'd a Language of their own, in which the Voyager communicated to his Mistress, how happy he should be to have her in his Country, where she should be Cloathed in such Silks as his Wastecoat was made of, and be carried in Houses drawn by Horses, without being exposed to Wind or Weather. All this he promised her the Enjoyment of, without such Fears and Alarms as they were there tormented with. In this tender Correspondence these Lovers lived for several Months, when Yarico, instructed by her Lover, discovered a Vessel on the Coast, to which she made Signals, and in the Night, with the utmost Joy and Satisfaction accompanied him to a Ships-Crew of his Country-Men, bound for Barbadoes. When a Vessel from the Main arrives in that Island, it seems the Planters come down to the Shoar, where there is an immediate Market of the Indians and other Slaves, as with us of Horses and Oxen.
     To be short, Mr. Thomas Inkle, now coming into English Territories, began seriously to reflect upon his loss of Time, and to weigh with himself how many Days Interest of his Mony he had lost during his Stay with Yarico. This Thought made the Young Man very pensive, and careful what Account he should be able to give his Friends of his Voyage. Upon which Considerations, the prudent and frugal young Man sold Yarico to a Barbadian Merchant; notwithstanding that the poor Girl, to incline him to commiserate her Condition, told him that she was with Child by him: But he only made use of that Information, to rise in his Demands upon the Purchaser.
 I was so touch'd with this Story, (which I think should be always a Counterpart to the Ephesian Matron) that I left the Room with Tears in my Eyes; which a Woman of Arietta's good Sense, did, I am sure, take for greater Applause, than any Compliments I could make her.
-R.
-</t>
+R.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -278,11 +274,10 @@
     We were invited to one of their publick Diversions, where we hoped to have seen the great Men of their Country running down a Stag or pitching a Bar, that we might have discovered who were the Persons of the greatest Abilities among them5; but instead of that, they conveyed us into a huge Room lighted up with abundance of Candles, where this lazy People sat still above three Hours to see several Feats of Ingenuity performed by others, who it seems were paid for it.
     As for the Women of the Country, not being able to talk with them, we could only make our Remarks upon them at a Distance. They let the Hair of their Heads grow to a great Length; but as the Men make a great Show with Heads of Hair that are not of their own, the Women, who they say have very fine Heads of Hair, tie it up in a Knot, and cover it from being seen. The Women look like Angels, and would be more beautiful than the Sun, were it not for little black Spots that are apt to break out in their Faces, and sometimes rise in very odd Figures. I have observed that those little Blemishes wear off very soon; but when they disappear in one Part of the Face, they are very apt to break out in another, insomuch that I have seen a Spot upon the Forehead in the Afternoon, which was upon the Chin in the Morning6.'
 The Author then proceeds to shew the Absurdity of Breeches and Petticoats, with many other curious Observations, which I shall reserve for another Occasion. I cannot however conclude this Paper without taking notice, That amidst these wild Remarks there now and then appears something very reasonable. I cannot likewise forbear observing, That we are all guilty in some Measure of the same narrow way of Thinking, which we meet with in this Abstract of the Indian Journal; when we fancy the Customs, Dress, and Manners of other Countries are ridiculous and extravagant, if they do not resemble those of our own.
-C.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Out of the innumerable Branches of mixt Wit, I shall choose one Instance which may be met with in all the Writers of this Class. The Passion of Love in its Nature has been thought to resemble Fire; for which Reason the Words Fire and Flame are made use of to signify Love. The witty Poets therefore have taken an Advantage from the doubtful Meaning of the Word Fire, to make an infinite Number of Witticisms. Cowley observing the cold Regard of his Mistress's Eyes, and at the same Time their Power of producing Love in him, considers them as Burning-Glasses made of Ice; and finding himself able to live in the greatest Extremities of Love, concludes the Torrid Zone to be habitable. When his Mistress has read his Letter written in Juice of Lemmon by holding it to the Fire, he desires her to read it over a second time by Love's Flames. When she weeps, he wishes it were inward Heat that distilled those Drops from the Limbeck. When she is absent he is beyond eighty, that is, thirty Degrees nearer the Pole than when she is with him. His ambitious Love is a Fire that naturally mounts upwards; his happy Love is the Beams of Heaven, and his unhappy Love Flames of Hell. When it does not let him sleep, it is a Flame that sends up no Smoak; when it is opposed by Counsel and Advice, it is a Fire that rages the more by the Wind's blowing upon it. Upon the dying of a Tree in which he had cut his Loves, he observes that his written Flames had burnt up and withered the Tree. When he resolves to give over his Passion, he tells us that one burnt like him for ever dreads the Fire. His Heart is an Ætna, that instead of Vulcan's Shop incloses Cupid's Forge in it. His endeavouring to drown his Love in Wine, is throwing Oil upon the Fire. He would insinuate to his Mistress, that the Fire of Love, like that of the Sun (which produces so many living Creatures) should not only warm but beget. Love in another Place cooks Pleasure at his Fire. Sometimes the Poet's Heart is frozen in every Breast, and sometimes scorched in every Eye. Sometimes he is drowned in Tears, and burnt in Love, like a Ship set on Fire in the Middle of the Sea.
+C.</t>
+  </si>
+  <si>
+    <t>Out of the innumerable Branches of mixt Wit, I shall choose one Instance which may be met with in all the Writers of this Class. The Passion of Love in its Nature has been thought to resemble Fire; for which Reason the Words Fire and Flame are made use of to signify Love. The witty Poets therefore have taken an Advantage from the doubtful Meaning of the Word Fire, to make an infinite Number of Witticisms. Cowley observing the cold Regard of his Mistress's Eyes, and at the same Time their Power of producing Love in him, considers them as Burning-Glasses made of Ice; and finding himself able to live in the greatest Extremities of Love, concludes the Torrid Zone to be habitable. When his Mistress has read his Letter written in Juice of Lemmon by holding it to the Fire, he desires her to read it over a second time by Love's Flames. When she weeps, he wishes it were inward Heat that distilled those Drops from the Limbeck. When she is absent he is beyond eighty, that is, thirty Degrees nearer the Pole than when she is with him. His ambitious Love is a Fire that naturally mounts upwards; his happy Love is the Beams of Heaven, and his unhappy Love Flames of Hell. When it does not let him sleep, it is a Flame that sends up no Smoak; when it is opposed by Counsel and Advice, it is a Fire that rages the more by the Wind's blowing upon it. Upon the dying of a Tree in which he had cut his Loves, he observes that his written Flames had burnt up and withered the Tree. When he resolves to give over his Passion, he tells us that one burnt like him for ever dreads the Fire. His Heart is an Ætna, that instead of Vulcan's Shop incloses Cupid's Forge in it. His endeavouring to drown his Love in Wine, is throwing Oil upon the Fire. He would insinuate to his Mistress, that the Fire of Love, like that of the Sun (which produces so many living Creatures) should not only warm but beget. Love in another Place cooks Pleasure at his Fire. Sometimes the Poet's Heart is frozen in every Breast, and sometimes scorched in every Eye. Sometimes he is drowned in Tears, and burnt in Love, like a Ship set on Fire in the Middle of the Sea.
 The Reader may observe in every one of these Instances, that the Poet mixes the Qualities of Fire with those of Love; and in the same Sentence speaking of it both as a Passion and as real Fire, surprizes the Reader with those seeming Resemblances or Contradictions that make up all the Wit in this kind of Writing. Mixt Wit therefore is a Composition of Punn and true Wit, and is more or less perfect as the Resemblance lies in the Ideas or in the Words: Its Foundations are laid partly in Falsehood and partly in Truth: Reason puts in her Claim for one Half of it, and Extravagance for the other. The only Province therefore for this kind of Wit, is Epigram, or those little occasional Poems that in their own Nature are nothing else but a Tissue of Epigrams. I cannot conclude this Head of mixt Wit, without owning that the admirable Poet out of whom I have taken the Examples of it, had as much true Wit as any Author that ever writ; and indeed all other Talents of an extraordinary Genius.
 It may be expected, since I am upon this Subject, that I should take notice of Mr. Dryden's Definition of Wit; which, with all the Deference that is due to the Judgment of so great a Man, is not so properly a Definition of Wit, as of good writing in general. Wit, as he defines it, is
     'a Propriety of Words and Thoughts adapted to the Subject.'2
@@ -292,8 +287,7 @@
 Were not I supported by so great an Authority as that of Mr. Dryden, I should not venture to observe, That the Taste of most of our English Poets, as well as Readers, is extremely Gothick. He quotes Monsieur Segrais7 for a threefold Distinction of the Readers of Poetry: In the first of which he comprehends the Rabble of Readers, whom he does not treat as such with regard to their Quality, but to their Numbers and Coarseness of their Taste. His Words are as follow:
     'Segrais has distinguished the Readers of Poetry, according to their Capacity of judging, into three Classes. [He might have said the same of Writers too, if he had pleased.] In the lowest Form he places those whom he calls Les Petits Esprits, such things as are our Upper-Gallery Audience in a Play-house; who like nothing but the Husk and Rind of Wit, prefer a Quibble, a Conceit, an Epigram, before solid Sense and elegant Expression: These are Mob Readers. If Virgil and Martial stood for Parliament-Men, we know already who would carry it. But though they make the greatest Appearance in the Field, and cry the loudest, the best on't is they are but a sort of French Huguenots, or Dutch Boors, brought over in Herds, but not Naturalized; who have not Lands of two Pounds per Annum in Parnassus, and therefore are not privileged to poll. Their Authors are of the same Level, fit to represent them on a Mountebank's Stage, or to be Masters of the Ceremonies in a Bear-garden: Yet these are they who have the most Admirers. But it often happens, to their Mortification, that as their Readers improve their Stock of Sense, (as they may by reading better Books, and by Conversation with Men of Judgment) they soon forsake them.'
 I must not dismiss this Subject without8 observing that as Mr. Lock in the Passage above-mentioned has discovered the most fruitful Source of Wit, so there is another of a quite contrary Nature to it, which does likewise branch it self out into several kinds. For not only the Resemblance, but the Opposition of Ideas, does very often produce Wit; as I could shew in several little Points, Turns and Antitheses, that I may possibly enlarge upon in some future Speculation.
-C.
-</t>
+C.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -310,8 +304,7 @@
     Fronde novâ puerum palumbes
     Texere ...
 I have heard that the late Lord Dorset, who had the greatest Wit temper'd with the greatest Candour,6 and was one of the finest Criticks as well as the best Poets of his Age, had a numerous collection of old English Ballads, and took a particular Pleasure in the Reading of them. I can affirm the same of Mr. Dryden, and know several of the most refined Writers of our present Age who are of the same Humour.
-I might likewise refer my Reader to Moliere's Thoughts on this Subject, as he has expressed them in the Character of the Misanthrope; but those only who are endowed with a true Greatness of Soul and Genius can divest themselves of the little Images of Ridicule, and admire Nature in her Simplicity and Nakedness. As for the little conceited Wits of the Age, who can only shew their Judgment by finding Fault, they cannot be supposed to admire these Productions which7 have nothing to recommend them but the Beauties of Nature, when they do not know how to relish even those Compositions that, with all the Beauties of Nature, have also the additional Advantages of Art8.
-</t>
+I might likewise refer my Reader to Moliere's Thoughts on this Subject, as he has expressed them in the Character of the Misanthrope; but those only who are endowed with a true Greatness of Soul and Genius can divest themselves of the little Images of Ridicule, and admire Nature in her Simplicity and Nakedness. As for the little conceited Wits of the Age, who can only shew their Judgment by finding Fault, they cannot be supposed to admire these Productions which7 have nothing to recommend them but the Beauties of Nature, when they do not know how to relish even those Compositions that, with all the Beauties of Nature, have also the additional Advantages of Art8.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -323,22 +316,20 @@
 I should not have been thus particular upon these ridiculous Horrours, did I not find them so very much prevail in all Parts of the Country. At the same time I think a Person who is thus terrify'd with the Imagination of Ghosts and Spectres much more reasonable than one who, contrary to the Reports of all Historians sacred and prophane, ancient and modern, and to the Traditions of all Nations, thinks the Appearance of Spirits fabulous and groundless: Could not I give myself up to this general Testimony of Mankind, I should to the Relations of particular Persons who are now living, and whom I cannot distrust in other Matters of Fact. I might here add, that not only the Historians, to whom we may join the Poets, but likewise the Philosophers of Antiquity have favoured this Opinion. Lucretius himself, though by the Course of his Philosophy he was obliged to maintain that the Soul did not exist separate from the Body, makes no Doubt of the Reality of Apparitions, and that Men have often appeared after their Death. This I think very remarkable; he was so pressed with the Matter of Fact which he could not have the Confidence to deny, that he was forced to account for it by one of the most absurd unphilosophical Notions that was ever started. He tells us, That the Surfaces of all Bodies are perpetually flying off from their respective Bodies, one after another; and that these Surfaces or thin Cases that included each other whilst they were joined in the Body like the Coats of an Onion, are sometimes seen entire when they are separated from it; by which means we often behold the Shapes and Shadows of Persons who are either dead or absent5.
 I shall dismiss this Paper with a Story out of Josephus, not so much for the sake of the Story it self as for the moral Reflections with which the Author concludes it, and which I shall here set down in his own Words.
     'Glaphyra the Daughter of King Archelaus, after the Death of her two first Husbands (being married to a third, who was Brother to her first Husband, and so passionately in love with her that he turned off his former Wife to make room for this Marriage) had a very odd kind of Dream. She fancied that she saw her first Husband coming towards her, and that she embraced him with great Tenderness; when in the midst of the Pleasure which she expressed at the Sight of him, he reproached her after the following manner: Glaphyra, says he, thou hast made good the old Saying, That Women are not to be trusted. Was not I the Husband of thy Virginity? Have I not Children by thee? How couldst thou forget our Loves so far as to enter into a second Marriage, and after that into a third, nay to take for thy Husband a Man who has so shamelessly crept into the Bed of his Brother? However, for the sake of our passed Loves, I shall free thee from thy present Reproach, and make thee mine for ever. Glaphyra told this Dream to several Women of her Acquaintance, and died soon after.6 I thought this Story might not be impertinent in this Place, wherein I speak of those Kings: Besides that, the Example deserves to be taken notice of as it contains a most certain Proof of the Immortality of the Soul, and of Divine Providence. If any Man thinks these Facts incredible, let him enjoy his own Opinion to himself, but let him not endeavour to disturb the Belief of others, who by Instances of this Nature are excited to the Study of Virtue.' 
-L.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I was taking a Walk in this Place last Night between the Hours of Nine and Ten, and could not but fancy it one of the most proper Scenes in the World for a Ghost to appear in. The Ruins of the Abby are scattered up and down on every Side, and half covered with Ivy and Elder-Bushes, the Harbours of several solitary Birds which seldom make their Appearance till the Dusk of the Evening. The Place was formerly a Churchyard, and has still several Marks in it of Graves and Burying-Places. There is such an Eccho among the old Ruins and Vaults, that if you stamp but a little louder than ordinary, you hear the Sound repeated. At the same time the Walk of Elms, with the Croaking of the Ravens which from time to time are heard from the Tops of them, looks exceeding solemn and venerable. These Objects naturally raise Seriousness and Attention; and when Night heightens the Awfulness of the Place, and pours out her supernumerary Horrors upon every thing in it, I do not at all wonder that weak Minds fill it with Spectres and Apparitions.
+L.</t>
+  </si>
+  <si>
+    <t>I was taking a Walk in this Place last Night between the Hours of Nine and Ten, and could not but fancy it one of the most proper Scenes in the World for a Ghost to appear in. The Ruins of the Abby are scattered up and down on every Side, and half covered with Ivy and Elder-Bushes, the Harbours of several solitary Birds which seldom make their Appearance till the Dusk of the Evening. The Place was formerly a Churchyard, and has still several Marks in it of Graves and Burying-Places. There is such an Eccho among the old Ruins and Vaults, that if you stamp but a little louder than ordinary, you hear the Sound repeated. At the same time the Walk of Elms, with the Croaking of the Ravens which from time to time are heard from the Tops of them, looks exceeding solemn and venerable. These Objects naturally raise Seriousness and Attention; and when Night heightens the Awfulness of the Place, and pours out her supernumerary Horrors upon every thing in it, I do not at all wonder that weak Minds fill it with Spectres and Apparitions.
 Mr. Locke, in his Chapter of the Association of Ideas, has very curious Remarks to shew how by the Prejudice of Education one Idea often introduces into the Mind a whole Set that bear no Resemblance to one another in the Nature of things. Among several Examples of this Kind, he produces the following Instance. The Ideas of Goblins and Sprights have really no more to do with Darkness than Light: Yet let but a foolish Maid inculcate these often on the Mind of a Child, and raise them there together, possibly he shall never be able to separate them again so long as he lives; but Darkness shall ever afterwards bring with it those frightful Ideas, and they shall be so joined, that he can no more bear the one than the other2.
 As I was walking in this Solitude, where the Dusk of the Evening conspired with so many other Occasions of Terrour, I observed a Cow grazing not far from me, which an Imagination that is apt to startle, might easily have construed into a black Horse without an Head: And I dare say the poor Footman lost his Wits upon some such trivial Occasion.
 My Friend Sir Roger has often told me with a great deal of Mirth, that at his first coming to his Estate he found three Parts of his House altogether useless; that the best Room in it had the Reputation of being haunted, and by that means was locked up; that Noises had been heard in his long Gallery, so that he could not get a Servant to enter it after eight a Clock at Night; that the Door of one of his Chambers was nailed up, because there went a Story in the Family that a Butler had formerly hang'd himself in it; and that his Mother, who lived to a great Age, had shut up half the Rooms in the House, in which either her Husband, a Son, or Daughter had died. The Knight seeing his Habitation reduced to3 so small a Compass, and himself in a manner shut out of his own House, upon the Death of his Mother ordered all the Apartments4 to be flung open, and exorcised by his Chaplain, who lay in every Room one after another, and by that Means dissipated the Fears which had so long reigned in the Family.
 I should not have been thus particular upon these ridiculous Horrours, did I not find them so very much prevail in all Parts of the Country. At the same time I think a Person who is thus terrify'd with the Imagination of Ghosts and Spectres much more reasonable than one who, contrary to the Reports of all Historians sacred and prophane, ancient and modern, and to the Traditions of all Nations, thinks the Appearance of Spirits fabulous and groundless: Could not I give myself up to this general Testimony of Mankind, I should to the Relations of particular Persons who are now living, and whom I cannot distrust in other Matters of Fact. I might here add, that not only the Historians, to whom we may join the Poets, but likewise the Philosophers of Antiquity have favoured this Opinion. Lucretius himself, though by the Course of his Philosophy he was obliged to maintain that the Soul did not exist separate from the Body, makes no Doubt of the Reality of Apparitions, and that Men have often appeared after their Death. This I think very remarkable; he was so pressed with the Matter of Fact which he could not have the Confidence to deny, that he was forced to account for it by one of the most absurd unphilosophical Notions that was ever started. He tells us, That the Surfaces of all Bodies are perpetually flying off from their respective Bodies, one after another; and that these Surfaces or thin Cases that included each other whilst they were joined in the Body like the Coats of an Onion, are sometimes seen entire when they are separated from it; by which means we often behold the Shapes and Shadows of Persons who are either dead or absent5.
 I shall dismiss this Paper with a Story out of Josephus, not so much for the sake of the Story it self as for the moral Reflections with which the Author concludes it, and which I shall here set down in his own Words.
     'Glaphyra the Daughter of King Archelaus, after the Death of her two first Husbands (being married to a third, who was Brother to her first Husband, and so passionately in love with her that he turned off his former Wife to make room for this Marriage) had a very odd kind of Dream. She fancied that she saw her first Husband coming towards her, and that she embraced him with great Tenderness; when in the midst of the Pleasure which she expressed at the Sight of him, he reproached her after the following manner: Glaphyra, says he, thou hast made good the old Saying, That Women are not to be trusted. Was not I the Husband of thy Virginity? Have I not Children by thee? How couldst thou forget our Loves so far as to enter into a second Marriage, and after that into a third, nay to take for thy Husband a Man who has so shamelessly crept into the Bed of his Brother? However, for the sake of our passed Loves, I shall free thee from thy present Reproach, and make thee mine for ever. Glaphyra told this Dream to several Women of her Acquaintance, and died soon after.6 I thought this Story might not be impertinent in this Place, wherein I speak of those Kings: Besides that, the Example deserves to be taken notice of as it contains a most certain Proof of the Immortality of the Soul, and of Divine Providence. If any Man thinks these Facts incredible, let him enjoy his own Opinion to himself, but let him not endeavour to disturb the Belief of others, who by Instances of this Nature are excited to the Study of Virtue.' 
-L.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. 146
+L.</t>
+  </si>
+  <si>
+    <t>No. 146
 Friday, August 17, 1711
 Steele
     Nemo Vir Magnus sine aliquo Afflatu divino unquam fuit.
@@ -346,8 +337,7 @@
 We know the highest Pleasure our Minds are capable of enjoying with Composure, when we read Sublime Thoughts communicated to us by Men of great Genius and Eloquence. Such is the Entertainment we meet with in the Philosophick Parts of Cicero's Writings. Truth and good Sense have there so charming a Dress, that they could hardly be more agreeably represented with the Addition of Poetical Fiction and the Power of Numbers. This ancient Author, and a modern one, had fallen into my Hands within these few Days; and the Impressions they have left upon me, have at the present quite spoiled me for a merry Fellow. The Modern is that admirable Writer the Author of The Theory of the Earth. The Subjects with which I have lately been entertained in them both bear a near Affinity; they are upon Enquiries into Hereafter, and the Thoughts of the latter seem to me to be raised above those of the former in proportion to his Advantages of Scripture and Revelation. If I had a Mind to it, I could not at present talk of any thing else; therefore I shall translate a Passage in the one, and transcribe a Paragraph out of the other, for the Speculation of this Day. Cicero tells us1, that Plato reports Socrates, upon receiving his Sentence, to have spoken to his Judges in the following manner.
     I have great Hopes, oh my Judges, that it is infinitely to my Advantage that I am sent to Death: For it is of necessity that one of these two things must be the Consequence. Death must take away all these Senses, or convey me to another Life. If all Sense is to be taken away, and Death is no more than that profound Sleep without Dreams, in which we are sometimes buried, oh Heavens! how desirable is it to die? how many Days do we know in Life preferable to such a State? But if it be true that Death is but a Passage to Places which they who lived before us do now inhabit, how much still happier is it to go from those who call themselves Judges, to appear before those that really are such; before Minos, Rhadamanthus, Æacus, and Triptolemus, and to meet Men who have lived with Justice and Truth? Is this, do you think, no happy Journey? Do you think it nothing to speak with Orpheus, Musceus, Homer, and Hesiod? I would, indeed, suffer many Deaths to enjoy these Things. With what particular Delight should I talk to Palamedes, Ajax, and others, who like me have suffered by the Iniquity of their Judges. I should examine the Wisdom of that great Prince, who carried such mighty Forces against Troy; and argue with Ulysses and Sisyphus, upon difficult Points, as I have in Conversation here, without being in Danger of being condemned. But let not those among you who have pronounced me an innocent Man be afraid of Death. No Harm can arrive at a good Man whether dead or living; his Affairs are always under the direction of the Gods; nor will I believe the Fate which is allotted to me myself this Day to have arrived by Chance; nor have I ought to say either against my Judges or Accusers, but that they thought they did me an Injury ... But I detain you too long, it is Time that I retire to Death, and you to your Affairs of Life; which of us has the Better is known to the Gods, but to no Mortal Man.
 The Divine Socrates is here represented in a Figure worthy his great Wisdom and Philosophy, worthy the greatest mere Man that ever breathed. But the modern Discourse is written upon a Subject no less than the Dissolution of Nature it self. Oh how glorious is the old Age of that great Man, who has spent his Time in such Contemplations as has made this Being, what only it should be, an Education for Heaven! He has, according to the Lights of Reason and Revelation, which seemed to him clearest, traced the Steps of Omnipotence: He has, with a Celestial Ambition, as far as it is consistent with Humility and Devotion, examined the Ways of Providence, from the Creation to the Dissolution of the visible World. How pleasing must have been the Speculation, to observe Nature and Providence move together, the Physical and Moral World march the same Pace: To observe Paradise and eternal Spring the Seat of Innocence, troubled Seasons and angry Skies the Portion of Wickedness and Vice. When this admirable Author has reviewed all that has past, or is to come, which relates to the habitable World, and run through the whole Fate of it, how could a Guardian Angel, that had attended it through all its Courses or Changes, speak more emphatically at the End of his Charge, than does our Author when he makes, as it were, a Funeral Oration over this Globe, looking to the Point where it once stood2?
-    Let us only, if you please, to take leave of this Subject, reflect upon this Occasion on the Vanity and transient Glory of this habitable World. How by the Force of one Element breaking loose upon the rest, all the Vanities of Nature, all the Works of Art, all the Labours of Men, are reduced to Nothing. All that we admired and adored before as great and magnificent, is obliterated or vanished; and another Form and Face of things, plain, simple, and every where the same, overspreads the whole Earth. Where are now the great Empires of the World, and their great Imperial Cities? Their Pillars, Trophies, and Monuments of Glory? Shew me where they stood, read the Inscription, tell me the Victors Name. What Remains, what Impressions, what Difference or Distinction, do you see in this Mass of Fire? Rome it self, eternal Rome, the great City, the Empress of the World, whose Domination and Superstition, ancient and modern, make a great Part of the History of the Earth, what is become of her now? She laid her Foundations deep, and her Palaces were strong and sumptuous; She glorified her self, and lived deliciously, and said in her Heart, I sit a Queen, and shall see no Sorrow: But her Hour is come, she is wiped away from the Face of the Earth, and buried in everlasting Oblivion. But it is not Cities only, and Works of Mens Hands, but the everlasting Hills, the Mountains and Rocks of the Earth are melted as Wax before the Sun, and their Place is no where found. Here stood the Alps, the Load of the Earth, that covered many Countries, and reached their Arms from the Ocean to the Black Sea; this huge Mass of Stone is softned and dissolved as a tender Cloud into Rain. Here stood the African Mountains, and Atlas with his Top above the Clouds; there was frozen Caucasus, and Taurus, and Imaus, and the Mountains of Asia; and yonder towards the North, stood the Riphaean Hills, cloathd in Ice and Snow. All these are Vanished, dropt away as the Snow upon their Heads. Great and Marvellous are thy Works, Just and True are thy Ways, thou King of Saints! Hallelujah. 
-</t>
+    Let us only, if you please, to take leave of this Subject, reflect upon this Occasion on the Vanity and transient Glory of this habitable World. How by the Force of one Element breaking loose upon the rest, all the Vanities of Nature, all the Works of Art, all the Labours of Men, are reduced to Nothing. All that we admired and adored before as great and magnificent, is obliterated or vanished; and another Form and Face of things, plain, simple, and every where the same, overspreads the whole Earth. Where are now the great Empires of the World, and their great Imperial Cities? Their Pillars, Trophies, and Monuments of Glory? Shew me where they stood, read the Inscription, tell me the Victors Name. What Remains, what Impressions, what Difference or Distinction, do you see in this Mass of Fire? Rome it self, eternal Rome, the great City, the Empress of the World, whose Domination and Superstition, ancient and modern, make a great Part of the History of the Earth, what is become of her now? She laid her Foundations deep, and her Palaces were strong and sumptuous; She glorified her self, and lived deliciously, and said in her Heart, I sit a Queen, and shall see no Sorrow: But her Hour is come, she is wiped away from the Face of the Earth, and buried in everlasting Oblivion. But it is not Cities only, and Works of Mens Hands, but the everlasting Hills, the Mountains and Rocks of the Earth are melted as Wax before the Sun, and their Place is no where found. Here stood the Alps, the Load of the Earth, that covered many Countries, and reached their Arms from the Ocean to the Black Sea; this huge Mass of Stone is softned and dissolved as a tender Cloud into Rain. Here stood the African Mountains, and Atlas with his Top above the Clouds; there was frozen Caucasus, and Taurus, and Imaus, and the Mountains of Asia; and yonder towards the North, stood the Riphaean Hills, cloathd in Ice and Snow. All these are Vanished, dropt away as the Snow upon their Heads. Great and Marvellous are thy Works, Just and True are thy Ways, thou King of Saints! Hallelujah.</t>
   </si>
   <si>
     <t xml:space="preserve">    ... Si quid ego adjuero, curamve levasso,
@@ -387,8 +377,7 @@
 Among innumerable Arguments which3 might be brought against such an unreasonable Proceeding, I shall only insist on one. We make it the Condition of our Forgiveness that we forgive others. In our very Prayers we desire no more than to be treated by this kind of Retaliation. The Case therefore before us seems to be what they call a Case in Point; the Relation between the Child and Father being what comes nearest to that between a Creature and its Creator. If the Father is inexorable to the Child who has offended, let the Offence be of never so high a Nature, how will he address himself to the Supreme Being under the tender Appellation of a Father, and desire of him such a Forgiveness as he himself refuses to grant?
 To this I might add many other religious, as well as many prudential Considerations; but if the last mentioned Motive does not prevail, I despair of succeeding by any other, and shall therefore conclude my Paper with a very remarkable Story, which is recorded in an old Chronicle published by Freher, among the Writers of the German History4.
 Eginhart, who was Secretary to Charles the Great, became exceeding popular by his Behaviour in that Post. His great Abilities gain'd him the Favour of his Master, and the Esteem of the whole Court. Imma, the Daughter of the Emperor, was so pleased with his Person and Conversation, that she fell in Love with him. As she was one of the greatest Beauties of the Age, Eginhart answer'd her with a more than equal Return of Passion. They stifled their Flames for some Time, under Apprehension of the fatal Consequences that might ensue. Eginhart at length resolving to hazard all, rather than be deprived of one whom his Heart was so much set upon, conveyed himself one Night into the Princess's Apartment, and knocking gently at the Door, was admitted as a Person who5 had something to communicate to her from the Emperor. He was with her in private most Part of the Night; but upon his preparing to go away about Break of Day, he observed that there had fallen a great Snow during his Stay with the Princess. This very much perplexed him, lest the Prints of his Feet in the Snow might make Discoveries to the King, who often used to visit his Daughter in the Morning. He acquainted the Princess Imma with his Fears; who, after some Consultations upon the Matter, prevailed upon him to let her carry him through the Snow upon her own Shoulders. It happened, that the Emperor not being able to sleep, was at that time up and walking in his Chamber, when upon looking through the Window he perceived his Daughter tottering under her Burden, and carrying his first Minister across the Snow; which she had no sooner done, but she returned again with the utmost Speed to her own Apartment. The Emperor was extreamly troubled and astonished at this Accident; but resolved to speak nothing of it till a proper Opportunity. In the mean time, Eginhart knowing that what he had done could not be long a Secret, determined to retire from Court; and in order to it begged the Emperor that he would be pleased to dismiss him, pretending a kind of Discontent at his not having been rewarded for his long Services. The Emperor would not give a direct Answer to his Petition, but told him he would think of it, and appointed6 a certain Day when he would let him know his Pleasure. He then called together the most faithful of his Counsellors, and acquainting them with his Secretary's Crime, asked them their Advice in so delicate an Affair. They most of them gave their Opinion, that the Person could not be too severely punished who had thus dishonoured his Master. Upon the whole Debate, the Emperor declared it was his Opinion, that Eginhart's Punishment would rather encrease than diminish the Shame of his Family, and that therefore he thought it the most adviseable to wear out the Memory of the Fact, by marrying him to his Daughter. Accordingly Eginhart was called in, and acquainted by the Emperor, that he should no longer have any Pretence of complaining his Services were not rewarded, for that the Princess Imma should be given him7 in Marriage, with a Dower suitable to her Quality; which was soon after performed accordingly.
-L.
-</t>
+L.</t>
   </si>
   <si>
     <t xml:space="preserve">    Plus aloës quàm mellis habet ...
@@ -448,8 +437,7 @@
 However that is, I humbly conceive the Business of a Levée is to receive the Acknowledgments of a Multitude, that a Man is Wise, Bounteous4, Valiant and Powerful. When the first Shot of Eyes is5 made, it is wonderful to observe how much Submission the Patron's Modesty can bear, and how much Servitude the Client's Spirit can descend to. In the vast Multiplicity of Business, and the Crowd about him, my Lord's Parts are usually so great, that, to the Astonishment of the whole Assembly, he has something to say to every Man there, and that so suitable to his Capacity, as any Man may judge that it is not without Talents that Men can arrive at great Employments. I have known a great Man ask a Flag-Officer, which way was the Wind, a Commander of Horse the present Price of Oats, and a Stock-jobber at what Discount such a Fund was, with as much Ease as if he had been bred to each of those several Ways of Life. Now this is extreamly obliging; for at the same time that the Patron informs himself of Matters, he gives the Person of whom he enquires an Opportunity to exert himself. What adds to the Pomp of those Interviews is, that it is performed with the greatest Silence and Order Imaginable. The Patron is usually in the midst of the Room, and some humble Person gives him a Whisper, which his Lordship answers aloud, It is well. Yes, I am of your Opinion. Pray inform yourself further, you may be sure of my Part in it. This happy Man is dismissed, and my Lord can turn himself to a Business of a quite different Nature, and offhand give as good an Answer as any great Man is obliged to. For the chief Point is to keep in Generals, and if there be any thing offered that's Particular, to be in haste.
 But we are now in the Height of the Affair, and my Lord's Creatures have all had their Whispers round to keep up the Farce of the thing, and the Dumb Show is become more general. He casts his Eye to that Corner, and there to Mr. such-a-one; to the other, and when did you come to Town? And perhaps just before he nods to another, and enters with him, but, Sir, I am glad to see you, now I think of it. Each of those are happy for the next four and twenty Hours; and those who bow in Ranks undistinguished, and by Dozens at a Time, think they have very good Prospects if they hope to arrive at such Notices half a Year hence.
 The Satyrist says6, there is seldom common Sense in high Fortune; and one would think, to behold a Levée, that the Great were not only infatuated with their Station, but also that they believed all below were seized too; else how is it possible that they could think of imposing upon themselves and others in such a degree, as to set up a Levée for any thing but a direct Farce? But such is the Weakness of our Nature, that when Men are a little exalted in their Condition, they immediately conceive they have additional Senses, and their Capacities enlarged not only above other Men, but above human Comprehension it self. Thus it is ordinary to see a great Man attend one listning, bow to one at a distance, and call to a third at the same instant. A Girl in new Ribbands is not more taken with her self, nor does she betray more apparent Coquetries, than even a wise Man in such a Circumstance of Courtship. I do not know any thing that I ever thought so very distasteful as the Affectation which is recorded of Cæsar, to wit, that he would dictate to three several Writers at the same time. This was an Ambition below the Greatness and Candour of his Mind. He indeed (if any Man had Pretensions to greater Faculties than any other Mortal) was the Person; but such a Way of acting is Childish, and inconsistent with the Manner of our Being. And it appears from the very Nature of Things, that there cannot be any thing effectually dispatched in the Distraction of a Publick Levée: but the whole seems to be a Conspiracy of a Set of Servile Slaves, to give up their own Liberty to take away their Patron's Understanding.
-T.
-</t>
+T.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -510,15 +498,14 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">It has been observed, his Blow is so well timed, that the most judicious Critick could never except against it. As soon as any shining Thought is expressed in the Poet, or any uncommon Grace appears in the Actor, he smites the Bench or Wainscot. If the Audience does not concur with him, he smites a second Time, and if the Audience is not yet awaked, looks round him with great Wrath, and repeats the Blow a third Time, which never fails to produce the Clap. He sometimes lets the Audience begin the Clap of themselves, and at the Conclusion of their Applause ratifies it with a single Thwack.
+    <t>It has been observed, his Blow is so well timed, that the most judicious Critick could never except against it. As soon as any shining Thought is expressed in the Poet, or any uncommon Grace appears in the Actor, he smites the Bench or Wainscot. If the Audience does not concur with him, he smites a second Time, and if the Audience is not yet awaked, looks round him with great Wrath, and repeats the Blow a third Time, which never fails to produce the Clap. He sometimes lets the Audience begin the Clap of themselves, and at the Conclusion of their Applause ratifies it with a single Thwack.
 He is of so great Use to the Play-house, that it is said a former Director of it, upon his not being able to pay his Attendance by reason of Sickness, kept one in Pay to officiate for him till such time as he recovered; but the Person so employed, tho' he laid about him with incredible Violence, did it in such wrong Places, that the Audience soon found out that it was not their old Friend the Trunk-maker.
 It has been remarked, that he has not yet exerted himself with Vigour this Season. He sometimes plies at the Opera; and upon Nicolini's first Appearance, was said to have demolished three Benches in the Fury of his Applause. He has broken half a dozen Oaken Plants upon Dogget1 and seldom goes away from a Tragedy of Shakespear, without leaving the Wainscot extremely shattered.
 The Players do not only connive at his obstreperous Approbation, but very cheerfully repair at their own Cost whatever Damages he makes. They had once a Thought of erecting a kind of Wooden Anvil for his Use that should be made of a very sounding Plank, in order to render his Stroaks more deep and mellow; but as this might not have been distinguished from the Musick of a Kettle-Drum, the Project was laid aside.
 In the mean while, I cannot but take notice of the great Use it is to an Audience, that a Person should thus preside over their Heads like the Director of a Consort, in order to awaken their Attention, and beat time to their Applauses; or, to raise my Simile, I have sometimes fancied the Trunk-maker in the upper Gallery to be like Virgils Ruler of the Wind, seated upon the Top of a Mountain, who, when he struck his Sceptre upon the Side of it, roused an Hurricane, and set the whole Cavern in an Uproar2.
 It is certain, the Trunk-maker has saved many a good Play, and brought many a graceful Actor into Reputation, who would not otherwise have been taken notice of. It is very visible, as the Audience is not a little abashed, if they find themselves betrayed into a Clap, when their Friend in the upper Gallery does not come into it; so the Actors do not value themselves upon the Clap, but regard it as a meer Brutum fulmen, or empty Noise, when it has not the Sound of the Oaken Plant in it. I know it has been given out by those who are Enemies to the Trunk-maker, that he has sometimes been bribed to be in the Interest of a bad Poet, or a vicious Player; but this is a Surmise which has no Foundation: his Stroaks are always just, and his Admonitions seasonable; he does not deal about his Blows at Random, but always hits the right Nail upon the Head. The3 inexpressible Force wherewith he lays them on, sufficiently shows the Evidence and Strength of his Conviction. His Zeal for a good Author is indeed outrageous, and breaks down every Fence and Partition, every Board and Plank, that stands within the Expression of his Applause.
 As I do not care for terminating my Thoughts in barren Speculations, or in Reports of pure Matter of Fact, without drawing something from them for the Advantage of my Countrymen, I shall take the Liberty to make an humble Proposal, that whenever the Trunk-maker shall depart this Life, or whenever he shall have lost the Spring of his Arm by Sickness, old Age, Infirmity, or the like, some able-bodied Critick should be advanced to this Post, and have a competent Salary settled on him for Life, to be furnished with Bamboos for Operas, Crabtree-Cudgels for Comedies, and Oaken Plants for Tragedy, at the publick Expence. And to the End that this Place should be always disposed of according to Merit, I would have none preferred to it, who has not given convincing Proofs both of a sound Judgment and a strong Arm, and who could not, upon Occasion, either knock down an Ox, or write a Comment upon Horace's Art of Poetry. In short, I would have him a due Composition of Hercules and Apollo, and so rightly qualified for this important Office, that the Trunk-maker may not be missed by our Posterity.
-C.
-</t>
+C.</t>
   </si>
   <si>
     <t xml:space="preserve">    Mr. Spectator,
@@ -700,8 +687,7 @@
 The Author here alludes to those Monuments of the Eastern Nations, which were Mountains of Stones raised upon the dead Body by Travellers, that used to cast every one his Stone upon it as they passed by. It is certain that no Monument is so glorious as one which is thus raised by the Hands of Envy. For my Part, I admire an Author for such a Temper of Mind as enables him to bear an undeserved Reproach without Resentment, more than for all the Wit of any the finest Satirical Reply.
 Thus far I thought necessary to explain my self in relation to those who have animadverted on this Paper, and to shew the Reasons why I have not thought fit to return them any formal Answer. I must further add, that the Work would have been of very little use to the Publick, had it been filled with personal Reflections and Debates; for which Reason I have never once turned out of my way to observe those little Cavils which have been made against it by Envy or Ignorance. The common Fry of Scriblers, who have no other way of being taken Notice of but by attacking what has gain'd some Reputation in the World, would have furnished me with Business enough, had they found me dispos'd to enter the Lists with them.
 I shall conclude with the Fable of Boccalini's Traveller, who was so pester'd with the Noise of Grasshoppers in his Ears, that he alighted from his Horse in great Wrath to kill them all. This, says the Author, was troubling himself to no manner of purpose: Had he pursued his Journey without taking notice of them, the troublesome Insects would have died of themselves in a very few Weeks, and he would have suffered nothing from them.
-L.
-</t>
+L.</t>
   </si>
   <si>
     <t xml:space="preserve">	
@@ -748,7 +734,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Gratian very often recommends the Fine Taste,1 as the utmost Perfection of an accomplished Man. As this Word arises very often in Conversation, I shall endeavour to give some Account of it, and to lay down Rules how we may know whether we are possessed of it, and how we may acquire that fine Taste of Writing, which is so much talked of among the Polite World.
+    <t>Gratian very often recommends the Fine Taste,1 as the utmost Perfection of an accomplished Man. As this Word arises very often in Conversation, I shall endeavour to give some Account of it, and to lay down Rules how we may know whether we are possessed of it, and how we may acquire that fine Taste of Writing, which is so much talked of among the Polite World.
 Most Languages make use of this Metaphor, to express that Faculty of the Mind, which distinguishes all the most concealed Faults and nicest Perfections in Writing. We may be sure this Metaphor would not have been so general in all Tongues, had there not been a very great Conformity between that Mental Taste, which is the Subject of this Paper, and that Sensitive Taste which gives us a Relish of every different Flavour that affects the Palate. Accordingly we find, there are as many Degrees of Refinement in the intellectual Faculty, as in the Sense, which is marked out by this common Denomination.
 I knew a Person who possessed the one in so great a Perfection, that after having tasted ten different Kinds of Tea, he would distinguish, without seeing the Colour of it, the particular Sort which was offered him; and not only so, but any two Sorts of them that were mixt together in an equal Proportion; nay he has carried the Experiment so far, as upon tasting the Composition of three different Sorts, to name the Parcels from whence the three several Ingredients were taken. A Man of a fine Taste in Writing will discern, after the same manner, not only the general Beauties and Imperfections of an Author, but discover the several Ways of thinking and expressing himself, which diversify him from all other Authors, with the several Foreign Infusions of Thought and Language, and the particular Authors from whom they were borrowed.
 After having thus far explained what is generally meant by a fine Taste in Writing, and shewn the Propriety of the Metaphor which is used on this Occasion, I think I may define it to be that Faculty of the Soul, which discerns the Beauties of an Author with Pleasure, and the Imperfections with Dislike. If a Man would know whether he is possessed of this Faculty, I would have him read over the celebrated Works of Antiquity, which have stood the Test of so many different Ages and Countries, or those Works among the Moderns which have the Sanction of the Politer Part of our Contemporaries. If upon the Perusal of such Writings he does not find himself delighted in an extraordinary Manner, or if, upon reading the admired Passages in such Authors, he finds a Coldness and Indifference in his Thoughts, he ought to conclude, not (as is too usual among tasteless Readers) that the Author wants those Perfections which have been admired in him, but that he himself wants the Faculty of discovering them.
@@ -759,8 +745,7 @@
 Conversation with Men of a Polite Genius is another Method for improving our Natural Taste. It is impossible for a Man of the greatest Parts to consider anything in its whole Extent, and in all its Variety of Lights. Every Man, besides those General Observations which are to be made upon an Author, forms several Reflections that are peculiar to his own Manner of Thinking; so that Conversation will naturally furnish us with Hints which we did not attend to, and make us enjoy other Men's Parts and Reflections as well as our own. This is the best Reason I can give for the Observation which several have made, that Men of great Genius in the same way of Writing seldom rise up singly, but at certain Periods of Time appear together, and in a Body; as they did at Rome in the Reign of Augustus, and in Greece about the Age of Socrates. I cannot think that Corneille, Racine, Moliere, Boileau, la Fontaine, Bruyere, Bossu, or the Daciers, would have written so well as they have done, had they not been Friends and Contemporaries.
 It is likewise necessary for a Man who would form to himself a finished Taste of good Writing, to be well versed in the Works of the best Criticks both Ancient and Modern. I must confess that I could wish there were Authors of this kind, who beside the Mechanical Rules which a Man of very little Taste may discourse upon, would enter into the very Spirit and Soul of fine Writing, and shew us the several Sources of that Pleasure which rises in the Mind upon the Perusal of a noble Work. Thus although in Poetry it be absolutely necessary that the Unities of Time, Place and Action, with other Points of the same Nature, should be thoroughly explained and understood; there is still something more essential to the Art, something that elevates and astonishes the Fancy, and gives a Greatness of Mind to the Reader, which few of the Criticks besides Longinus have considered.
 Our general Taste in England is for Epigram, Turns of Wit, and forced Conceits, which have no manner of Influence, either for the bettering or enlarging the Mind of him who reads them, and have been carefully avoided by the greatest Writers, both among the Ancients and Moderns. I have endeavoured in several of my Speculations to banish this Gothic Taste, which has taken Possession among us. I entertained the Town, for a Week together, with an Essay upon Wit, in which I endeavoured to detect several of those false Kinds which have been admired in the different Ages of the World; and at the same time to shew wherein the Nature of true Wit consists. I afterwards gave an Instance of the great Force which lyes in a natural Simplicity of Thought to affect the Mind of the Reader, from such vulgar Pieces as have little else besides this single Qualification to recommend them. I have likewise examined the Works of the greatest Poet which our Nation or perhaps any other has produced, and particularized most of those rational and manly Beauties which give a Value to that Divine Work. I shall next Saturday enter upon an Essay on the Pleasures of the Imagination, which, though it shall consider that Subject at large, will perhaps suggest to the Reader what it is that gives a Beauty to many Passages of the finest Writers both in Prose and Verse. As an Undertaking of this Nature is entirely new, I question not but it will be received with Candour.
-O.
-</t>
+O.</t>
   </si>
   <si>
     <t xml:space="preserve">    Avia Pieridum peragro loca, nullius ante
@@ -788,8 +773,7 @@
 In the like manner, when we read of Torments, Wounds, Deaths, and the like dismal Accidents, our Pleasure does not flow so properly from the Grief which such melancholy Descriptions give us, as from the secret Comparison which we make between our selves and the Person who2 suffers. Such Representations teach us to set a just Value upon our own Condition, and make us prize our good Fortune, which exempts us from the like Calamities. This is, however, such a kind of Pleasure as we are not capable of receiving, when we see a Person actually lying under the Tortures that we meet with in a Description; because in this case, the Object presses too close upon our Senses, and bears so hard upon us, that it does not give us Time or Leisure to reflect on our selves. Our Thoughts are so intent upon the Miseries of the Sufferer, that we cannot turn them upon our own Happiness. Whereas, on the contrary, we consider the Misfortunes we read in History or Poetry, either as past, or as fictitious, so that the Reflection upon our selves rises in us insensibly, and over-bears the Sorrow we conceive for the Sufferings of the Afflicted.
 But because the Mind of Man requires something more perfect in Matter, than what it finds there, and can never meet with any Sight in Nature which sufficiently answers its highest Ideas of Pleasantness; or, in other Words, because the Imagination can fancy to it self Things more Great, Strange, or Beautiful, than the Eye ever saw, and is still sensible of some Defect in what it has seen; on this account it is the part of a Poet to humour the Imagination in its own Notions, by mending and perfecting Nature where he describes a Reality, and by adding greater Beauties than are put together in Nature, where he describes a Fiction.
 He is not obliged to attend her in the slow Advances which she makes from one Season to another, or to observe her Conduct, in the successive Production of Plants and Flowers. He may draw into his Description all the Beauties of the Spring and Autumn, and make the whole Year contribute something to render it the more agreeable. His Rose-trees, Wood-bines, and Jessamines may flower together, and his Beds be cover'd at the same time with Lillies, Violets, and Amaranths. His Soil is not restrained to any particular Sett of Plants, but is proper either for Oaks or Mirtles, and adapts itself to the Products of every Climate. Oranges may grow wild in it; Myrrh may be met with in every Hedge, and if he thinks it proper to have a Grove of Spices, he can quickly command Sun enough to raise it. If all this will not furnish out an agreeable Scene, he can make several new Species of Flowers, with richer Scents and higher Colours than any that grow in the Gardens of Nature. His Consorts of Birds may be as full and harmonious, and his Woods as thick and gloomy as he pleases. He is at no more Expence in a long Vista, than a short one, and can as easily throw his Cascades from a Precipice of half a Mile high, as from one of twenty Yards. He has his Choice of the Winds, and can turn the Course of his Rivers in all the Variety of Meanders, that are most delightful to the Reader's Imagination. In a word, he has the modelling of Nature in his own Hands, and may give her what Charms he pleases, provided he does not reform her too much, and run into Absurdities, by endeavouring to excel.
-O.
-</t>
+O.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -803,8 +787,7 @@
 In the like manner, when we read of Torments, Wounds, Deaths, and the like dismal Accidents, our Pleasure does not flow so properly from the Grief which such melancholy Descriptions give us, as from the secret Comparison which we make between our selves and the Person who2 suffers. Such Representations teach us to set a just Value upon our own Condition, and make us prize our good Fortune, which exempts us from the like Calamities. This is, however, such a kind of Pleasure as we are not capable of receiving, when we see a Person actually lying under the Tortures that we meet with in a Description; because in this case, the Object presses too close upon our Senses, and bears so hard upon us, that it does not give us Time or Leisure to reflect on our selves. Our Thoughts are so intent upon the Miseries of the Sufferer, that we cannot turn them upon our own Happiness. Whereas, on the contrary, we consider the Misfortunes we read in History or Poetry, either as past, or as fictitious, so that the Reflection upon our selves rises in us insensibly, and over-bears the Sorrow we conceive for the Sufferings of the Afflicted.
 But because the Mind of Man requires something more perfect in Matter, than what it finds there, and can never meet with any Sight in Nature which sufficiently answers its highest Ideas of Pleasantness; or, in other Words, because the Imagination can fancy to it self Things more Great, Strange, or Beautiful, than the Eye ever saw, and is still sensible of some Defect in what it has seen; on this account it is the part of a Poet to humour the Imagination in its own Notions, by mending and perfecting Nature where he describes a Reality, and by adding greater Beauties than are put together in Nature, where he describes a Fiction.
 He is not obliged to attend her in the slow Advances which she makes from one Season to another, or to observe her Conduct, in the successive Production of Plants and Flowers. He may draw into his Description all the Beauties of the Spring and Autumn, and make the whole Year contribute something to render it the more agreeable. His Rose-trees, Wood-bines, and Jessamines may flower together, and his Beds be cover'd at the same time with Lillies, Violets, and Amaranths. His Soil is not restrained to any particular Sett of Plants, but is proper either for Oaks or Mirtles, and adapts itself to the Products of every Climate. Oranges may grow wild in it; Myrrh may be met with in every Hedge, and if he thinks it proper to have a Grove of Spices, he can quickly command Sun enough to raise it. If all this will not furnish out an agreeable Scene, he can make several new Species of Flowers, with richer Scents and higher Colours than any that grow in the Gardens of Nature. His Consorts of Birds may be as full and harmonious, and his Woods as thick and gloomy as he pleases. He is at no more Expence in a long Vista, than a short one, and can as easily throw his Cascades from a Precipice of half a Mile high, as from one of twenty Yards. He has his Choice of the Winds, and can turn the Course of his Rivers in all the Variety of Meanders, that are most delightful to the Reader's Imagination. In a word, he has the modelling of Nature in his own Hands, and may give her what Charms he pleases, provided he does not reform her too much, and run into Absurdities, by endeavouring to excel.
-O.
-</t>
+O.</t>
   </si>
   <si>
     <t xml:space="preserve">	
@@ -833,8 +816,7 @@
 Paper IX 	Of that kind of Poetry which Mr. Dryden calls the Fairy Way of Writing. How a Poet should be Qualified for it. The Pleasures of the Imagination that arise from it. In this respect why the Moderns excell the Ancients. Why the English excell the Moderns. Who the Best among the English. Of Emblematical Persons.
 Paper X 	What Authors please the Imagination who have nothing to do with Fiction. How History pleases the Imagination. How the Authors of the new Philosophy please the Imagination. The Bounds and Defects of the Imagination. Whether these Defects are Essential to the Imagination.
 Paper XI 	How those please the Imagination who treat of Subjects abstracted from Matter, by Allusions taken from it. What Allusions most pleasing to the Imagination. Great Writers how Faulty in this Respect. Of the Art of Imagining in General. The Imagination capable of Pain as well as Pleasure. In what Degree the Imagination is capable either of Pain or Pleasure.
-O.
-</t>
+O.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -848,8 +830,7 @@
 Paper IX 	Of that kind of Poetry which Mr. Dryden calls the Fairy Way of Writing. How a Poet should be Qualified for it. The Pleasures of the Imagination that arise from it. In this respect why the Moderns excell the Ancients. Why the English excell the Moderns. Who the Best among the English. Of Emblematical Persons.
 Paper X 	What Authors please the Imagination who have nothing to do with Fiction. How History pleases the Imagination. How the Authors of the new Philosophy please the Imagination. The Bounds and Defects of the Imagination. Whether these Defects are Essential to the Imagination.
 Paper XI 	How those please the Imagination who treat of Subjects abstracted from Matter, by Allusions taken from it. What Allusions most pleasing to the Imagination. Great Writers how Faulty in this Respect. Of the Art of Imagining in General. The Imagination capable of Pain as well as Pleasure. In what Degree the Imagination is capable either of Pain or Pleasure.
-O.
-</t>
+O.</t>
   </si>
   <si>
     <t xml:space="preserve">    Est natura Hominum Novitatis avida.
@@ -881,7 +862,7 @@
     They advise from Fulham, that things remained there in the same State they were. They had Intelligence, just as the Letters came away, of a Tub of excellent Ale just set abroach at Parson's Green; but this wanted Confirmation.</t>
   </si>
   <si>
-    <t xml:space="preserve">We may likewise observe in the third Place, that the Passions affect the Mind with greater Strength when we are asleep, than when we are awake. Joy and Sorrow give us more vigorous Sensations of Pain or Pleasure at this time, than at any other. Devotion likewise, as the excellent Author above-mentioned has hinted, is in a very particular manner heightned and inflamed, when it rises in the Soul at a time that the Body is thus laid at Rest. Every Man's Experience will inform him in this matter, though it is very probable, that this may happen differently, in different Constitutions. I shall conclude this Head with the two following Problems, which I shall leave to the Solution of my Reader. Supposing a Man always happy in his Dreams, and miserable in his waking Thoughts, and that his Life was equally divided between them, whether would he be more happy or miserable? Were a Man a King in his Dreams, and a Beggar awake, and dreamt as consequentially, and in as continued unbroken Schemes as he thinks when awake, whether he would be in reality a King or Beggar, or rather whether he would not be both?
+    <t>We may likewise observe in the third Place, that the Passions affect the Mind with greater Strength when we are asleep, than when we are awake. Joy and Sorrow give us more vigorous Sensations of Pain or Pleasure at this time, than at any other. Devotion likewise, as the excellent Author above-mentioned has hinted, is in a very particular manner heightned and inflamed, when it rises in the Soul at a time that the Body is thus laid at Rest. Every Man's Experience will inform him in this matter, though it is very probable, that this may happen differently, in different Constitutions. I shall conclude this Head with the two following Problems, which I shall leave to the Solution of my Reader. Supposing a Man always happy in his Dreams, and miserable in his waking Thoughts, and that his Life was equally divided between them, whether would he be more happy or miserable? Were a Man a King in his Dreams, and a Beggar awake, and dreamt as consequentially, and in as continued unbroken Schemes as he thinks when awake, whether he would be in reality a King or Beggar, or rather whether he would not be both?
 There is another Circumstance, which methinks gives us a very high Idea of the Nature of the Soul, in regard to what passes in Dreams, I mean that innumerable Multitude and Variety of Ideas which then arise in her. Were that active watchful Being only conscious of her own Existence at such a time, what a painful Solitude would her Hours of Sleep be? Were the Soul sensible of her being alone in her sleeping Moments, after the same manner that she is sensible of it while awake, the time would hang very heavy on her, as it often actually does when she Dreams that she is in such a Solitude?
     —Semperque relinqui
     Sola sili, semper longam incomitata videtur
@@ -891,8 +872,7 @@
 I must not omit that Argument for the Excellency of the Soul, which I have seen quoted out of Tertullian3, namely, its Power of divining in Dreams. That several such Divinations have been made, none can question, who believes the Holy Writings, or who has but the least degree of a common Historical Faith; there being innumerable Instances of this nature in several Authors, both Antient and Modern, Sacred and Profane. Whether such dark Presages, such Visions of the Night proceed from any latent Power in the Soul, during this her state of Abstraction, or from any Communication with the Supreme Being, or from any operation of Subordinate Spirits, has been a great Dispute among the Learned; the matter of Fact is, I think, incontestable, and has been looked upon as such by the greatest Writers, who have been never suspected either of Superstition or Enthusiasm.
 I do not suppose, that the Soul in these Instances is entirely loose and unfettered from the Body: It is sufficient, if she is not so far sunk, and immersed in Matter, nor intangled and perplexed in her Operations, with such Motions of Blood and Spirits, as when she actuates the Machine in its waking Hours. The Corporeal Union is slackned enough to give the Mind more Play. The Soul seems gathered within herself, and recovers that Spring which is broke and weakned, when she operates more in concert with the Body.
 The Speculations I have here made, if they are not Arguments, they are at least strong Intimations, not only of the Excellency of an Human Soul, but of its Independence on the Body; and if they do not prove, do at least confirm these two great Points, which are established by many other Reasons that are altogether unanswerable.
-O.
-</t>
+O.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -904,8 +884,7 @@
     Sir ,
     Your most humble Servant,
     Ralph Wonder.
-T.
-</t>
+T.</t>
   </si>
   <si>
     <t xml:space="preserve">	
@@ -938,15 +917,14 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">I am always highly delighted with the discovery of any rising Genius among my Countrymen. For this reason I have read over, with great pleasure, the late Miscellany published by Mr. Pope1, in which there are many excellent Compositions of that ingenious Gentleman. I have had a pleasure of the same kind, in perusing a Poem that is just publish'd on the Prospect of Peace, and which, I hope, will meet with such a Reward from its Patrons, as so noble a Performance deserves. I was particularly well pleased to find that the Author had not amused himself with Fables out of the Pagan Theology, and that when he hints at any thing of this2 nature, he alludes to it only as to a Fable.
+    <t>I am always highly delighted with the discovery of any rising Genius among my Countrymen. For this reason I have read over, with great pleasure, the late Miscellany published by Mr. Pope1, in which there are many excellent Compositions of that ingenious Gentleman. I have had a pleasure of the same kind, in perusing a Poem that is just publish'd on the Prospect of Peace, and which, I hope, will meet with such a Reward from its Patrons, as so noble a Performance deserves. I was particularly well pleased to find that the Author had not amused himself with Fables out of the Pagan Theology, and that when he hints at any thing of this2 nature, he alludes to it only as to a Fable.
 Many of our Modern Authors, whose Learning very often extends no farther than Ovid's Metamorphosis, do not know how to celebrate a Great Man, without mixing a parcel of School-Boy Tales with the Recital of his Actions. If you read a Poem on a fine Woman, among the Authors of this Class, you shall see that it turns more upon Venus or Helen, that on the Party concerned. I have known a Copy of Verses on a great Hero highly commended; but upon asking to hear some of the beautiful Passages, the Admirer of it has repeated to me a Speech of Apollo, or a Description of Polypheme. At other times when I have search'd for the Actions of a great Man, who gave a Subject to the Writer, I have been entertained with the Exploits of a River-God, or have been forced to attend a Fury in her mischievous Progress, from one end of the Poem to the other. When we are at School it is necessary for us to be acquainted with the System of Pagan Theology, and may be allowed to enliven a Theme, or point an Epigram with an Heathen God; but when we would write a manly Panegyrick, that should carry in it all the Colours of Truth, nothing can be more ridiculous than to have recourse to our Jupiters and Junos.
 No Thought is beautiful which is not just, and no Thought can be just which is not founded in Truth, or at least in that which passes for such.
 In Mock-Heroick Poems, the Use of the Heathen Mythology is not only excusable but graceful, because it is the Design of such Compositions to divert, by adapting the fabulous Machines of the Ancients to low Subjects, and at the same time by ridiculing such kinds of Machinery in modern Writers. If any are of opinion, that there is a Necessity of admitting these Classical Legends into our serious Compositions, in order to give them a more Poetical Turn; I would recommend to their Consideration the Pastorals of Mr. Philips. One would have thought it impossible for this Kind of Poetry to have subsisted without Fawns and Satyrs, Wood Nymphs, and Water Nymphs, with all the Tribe of rural Deities. But we see he has given a new Life, and a more natural Beauty to this way of Writing by substituting in the place of these Antiquated Fables, the superstitious Mythology which prevails among the Shepherds of our own Country.
 Virgil and Homer might compliment their Heroes, by interweaving the Actions of Deities with their Atchievements; but for a Christian Author to write in the Pagan Creed, to make Prince Eugene a Favourite of Mars, or to carry on a Correspondence between Bellona and the Marshal de Villars, would be downright Puerility, and unpardonable in a Poet that is past Sixteen. It is want of sufficient Elevation in a Genius to describe Realities, and place them in a shining Light, that makes him have recourse to such trifling antiquated Fables; as a Man may write a fine Description of Bacchus or Apollo, that does not know how to draw the Character of any of his Contemporaries.
 In order therefore to put a stop to this absurd Practice, I shall publish the following Edict, by virtue of that Spectatorial Authority with which I stand invested.
 'Whereas the Time of a General Peace is, in all appearance, drawing near, being inform'd that there are several ingenious Persons who intend to shew their Talents on so happy an Occasion, and being willing, as much as in me lies, to prevent that Effusion of Nonsense, which we have good Cause to apprehend; I do hereby strictly require every Person, who shall write on this Subject, to remember that he is a Christian, and not to Sacrifice his Catechism to his Poetry. In order to it, I do expect of him in the first place, to make his own Poem, without depending upon Phœbus for any part of it, or calling out for Aid upon any one of the Muses by Name. I do likewise positively forbid the sending of Mercury with any particular Message or Dispatch relating to the Peace, and shall by no means suffer Minerva to take upon her the Shape of any Plenipotentiary concerned in this Great Work. I do further declare, that I shall not allow the Destinies to have had an hand in the Deaths of the several thousands who have been slain in the late War, being of opinion that all such Deaths may be very well accounted for by the Christian System of Powder and Ball. I do therefore strictly forbid the Fates to cut the Thread of Man's Life upon any pretence whatsoever, unless it be for the sake of the Rhyme. And whereas I have good Reason to fear, that Neptune will have a great deal of Business on his Hands, in several Poems which we may now suppose are upon the Anvil, I do also prohibit his Appearance, unless it be done in Metaphor, Simile, or any very short Allusion, and that even here he be not permitted to enter, but with great Caution and Circumspection. I deSir e that the same Rule may be extended to his whole Fraternity of Heathen Gods, it being my design to condemn every Poem to the Flames in which Jupiter Thunders, or exercises any other Act of Authority which does not belong to him: In short, I expect that no Pagan Agent shall be introduc'd, or any Fact related which a Man cannot give Credit to with a good Conscience. Provided always, that nothing herein contained shall extend, or be construed to extend, to several of the Female Poets in this Nation, who shall be still left in full Possession of their Gods and Goddesses, in the same manner as if this Paper had never been written.
-O.
-</t>
+O.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1006,15 +984,14 @@
 I am,</t>
   </si>
   <si>
-    <t xml:space="preserve">The most violent Egotism which I have met with in the Course of my Reading, is that of Cardinal Wolsey, Ego et Rex meus, I and my King; as perhaps the most eminent Egotist that ever appeared in the World, was Montagne the Author of the celebrated Essays. This lively old Gascon has woven all his bodily Infirmities into his Works, and after having spoken of the Faults or Virtues of any other Man, immediately publishes to the World how it stands with himself in that Particular. Had he kept his own Counsel he might have passed for a much better Man, though perhaps he would not have been so diverting an Author. The Title of an Essay promises perhaps a Discourse upon Virgil or Julius Cæsar; but when you look into it, you are sure to meet with more upon Monsieur Montagne, than of either of them. The younger Scaliger, who seems to have been no great Friend to this Author, after having acquainted the World that his Father sold Herrings, adds these Words;
+    <t>The most violent Egotism which I have met with in the Course of my Reading, is that of Cardinal Wolsey, Ego et Rex meus, I and my King; as perhaps the most eminent Egotist that ever appeared in the World, was Montagne the Author of the celebrated Essays. This lively old Gascon has woven all his bodily Infirmities into his Works, and after having spoken of the Faults or Virtues of any other Man, immediately publishes to the World how it stands with himself in that Particular. Had he kept his own Counsel he might have passed for a much better Man, though perhaps he would not have been so diverting an Author. The Title of an Essay promises perhaps a Discourse upon Virgil or Julius Cæsar; but when you look into it, you are sure to meet with more upon Monsieur Montagne, than of either of them. The younger Scaliger, who seems to have been no great Friend to this Author, after having acquainted the World that his Father sold Herrings, adds these Words;
     La grande fadaise de Montague, qui a escrit, qu'il aimoit mieux le vin blanc—que diable a-t-on a faire de scavoir ce qu'il aime? For my Part, says Montague, I am a great Lover of your White Wines—What the Devil signifies it to the Publick, says Scaliger, whether he is a Lover of White Wines or of Red Wines?
 I cannot here forbear mentioning a Tribe of Egotists for whom I have always had a mortal Aversion, I mean the Authors of Memoirs, who are never mentioned in any Works but their own, and who raise all their Productions out of this single Figure of Speech.
 Most of our modern Prefaces savour very strongly of the Egotism. Every insignificant Author fancies it of Importance to the World, to know that he writ his Book in the Country, that he did it to pass away some of his idle Hours, that it was published at the Importunity of Friends, or that his natural Temper, Studies or Conversations, directed him to the Choice of his Subject.
     —Id populus curat scilicet.
 Such Informations cannot but be highly improving to the Reader.
 In Works of Humour, especially when a Man writes under a fictitious Personage, the talking of one's self may give some Diversion to the Publick; but I would advise every other Writer never to speak of himself, unless there be something very considerable in his Character: Tho' I am sensible this Rule will be of little Use in the World, because there is no Man who fancies his Thoughts worth publishing, that does not look upon himself as a considerable Person.
-I shall close this Paper with a Remark upon such as are Egotists in Conversation: These are generally the vain or shallow part of Mankind, People being naturally full of themselves when they have nothing else in them. There is one kind of Egotists which is very common in the World, tho' I do not remember that any Writer has taken Notice of them; I mean those empty conceited Fellows, who repeat as Sayings of their own, or some of their particular Friends, several Jests which were made before they were born, and which every one who has conversed in the World has heard a hundred times over. A forward young Fellow of my Acquaintance was very guilty of this Absurdity: He would be always laying a new Scene for some old Piece of Wit, and telling us, That as he and Jack such-a-one were together, one or t'other of them had such a Conceit on such an Occasion; upon which he would laugh very heartily, and wonder the Company did not join with him. When his Mirth was over, I have often reprehended him out of Terence, Tuumne, obsecro te, hoc dictum erat? vetus credidi. But finding him still incorrigible, and having a Kindness for the young Coxcomb, who was otherwise a good-natured Fellow, I recommended to his Perusal the Oxford and Cambridge Jests, with several little Pieces of Pleasantry of the same Nature. Upon the reading of them, he was under no small Confusion to find that all his Jokes had passed through several Editions, and that what he thought was a new Conceit, and had appropriated to his own Use, had appeared in Print before he or his ingenious Friends were ever heard of. This had so good an Effect upon him, that he is content at present to pass for a Man of plain Sense in his ordinary Conversation, and is never facetious but when he knows his Company.
-</t>
+I shall close this Paper with a Remark upon such as are Egotists in Conversation: These are generally the vain or shallow part of Mankind, People being naturally full of themselves when they have nothing else in them. There is one kind of Egotists which is very common in the World, tho' I do not remember that any Writer has taken Notice of them; I mean those empty conceited Fellows, who repeat as Sayings of their own, or some of their particular Friends, several Jests which were made before they were born, and which every one who has conversed in the World has heard a hundred times over. A forward young Fellow of my Acquaintance was very guilty of this Absurdity: He would be always laying a new Scene for some old Piece of Wit, and telling us, That as he and Jack such-a-one were together, one or t'other of them had such a Conceit on such an Occasion; upon which he would laugh very heartily, and wonder the Company did not join with him. When his Mirth was over, I have often reprehended him out of Terence, Tuumne, obsecro te, hoc dictum erat? vetus credidi. But finding him still incorrigible, and having a Kindness for the young Coxcomb, who was otherwise a good-natured Fellow, I recommended to his Perusal the Oxford and Cambridge Jests, with several little Pieces of Pleasantry of the same Nature. Upon the reading of them, he was under no small Confusion to find that all his Jokes had passed through several Editions, and that what he thought was a new Conceit, and had appropriated to his own Use, had appeared in Print before he or his ingenious Friends were ever heard of. This had so good an Effect upon him, that he is content at present to pass for a Man of plain Sense in his ordinary Conversation, and is never facetious but when he knows his Company.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1031,7 +1008,7 @@
     'I set it down, and drew out another, in which I took the Fomes at first Sight to be very small, but was amazed to find, that as I looked stedfastly upon it, it grew still larger. It was the Heart of Melissa, a noted Prude who lives the next Door to me.</t>
   </si>
   <si>
-    <t xml:space="preserve">One of the first that talked in this lofty Strain of our Nature was Beneficence, would his Followers say, is all founded in Weakness; and, whatever be pretended, the Kindness that passeth between Men and Men is by every Man directed to himself. This, it must be confessed, is of a Piece with the rest of that hopeful Philosophy, which having patch'd Man up out of the four Elements, attributes his Being to Chance, and derives all his Actions from an unintelligible Declination of Atoms. And for these glorious Discoveries the Poet is beyond Measure transported in the Praises of his Hero, as if he must needs be something more than Man, only for an Endeavour to prove that Man is in nothing superior to Beasts.
+    <t>One of the first that talked in this lofty Strain of our Nature was Beneficence, would his Followers say, is all founded in Weakness; and, whatever be pretended, the Kindness that passeth between Men and Men is by every Man directed to himself. This, it must be confessed, is of a Piece with the rest of that hopeful Philosophy, which having patch'd Man up out of the four Elements, attributes his Being to Chance, and derives all his Actions from an unintelligible Declination of Atoms. And for these glorious Discoveries the Poet is beyond Measure transported in the Praises of his Hero, as if he must needs be something more than Man, only for an Endeavour to prove that Man is in nothing superior to Beasts.
 In this School was Mr. Hobs instructed to speak after the same Manner, if he did not rather draw his Knowledge from an Observation of his own Temper; for he somewhere unluckily lays down this as a Rule,
     'That from the Similitudes of Thoughts and Passions of one Man to the Thoughts and Passions of another, whosoever looks into himself and considers what he doth when he thinks, hopes, fears, &amp;c., and upon what Grounds; he shall hereby read and know what are the Thoughts and Passions of all other Men upon the like Occasions.'
 Now we will allow Mr. Hobs to know best how he was inclined; But in earnest, I should be heartily out of Conceit with my self, if I thought my self of this unamiable Temper, as he affirms, and should have as little Kindness for my self as for any Body in the World. Hitherto I always imagined that kind and benevolent Propensions were the original Growth of the Heart of Man, and, however checked and over-topped by counter Inclinations that have since sprung up within us, have still some Force in the worst of Tempers, and a considerable Influence on the best. And, methinks, it's a fair Step towards the Proof of this, that the most beneficent of all Beings is He who hath an absolute Fulness of Perfection in Himself, who gave Existence to the Universe, and so cannot be supposed to want that which He communicated, without diminishing from the Plenitude of his own Power and Happiness. The Philosophers before mentioned have indeed done all that in them lay to invalidate this Argument; for, placing the Gods in a State of the most elevated Blessedness, they describe them as Selfish as we poor miserable Mortals can be, and shut them out from all Concern for Mankind, upon the Score of their having no Need of us.
@@ -1040,8 +1017,7 @@
 But to descend from Reason to Matter of Fact; the Pity which arises on Sight of Persons in Distress, and the Satisfaction of Mind which is the Consequence of having removed them into a happier State, are instead of a thousand Arguments to prove such a thing as a disinterested Benevolence. Did Pity proceed from a Reflection we make upon our Liableness to the same ill Accidents we see befall others, it were nothing to the present Purpose; but this is assigning an artificial Cause of a natural Passion, and can by no Means be admitted as a tolerable Account of it, because Children and Persons most Thoughtless about their own Condition, and incapable of entering into the Prospects of Futurity, feel the most violent Touches of Compassion.
 And then as to that charming Delight which immediately follows the giving Joy to another, or relieving his Sorrow, and is, when the Objects are numerous, and the kindness of Importance really inexpressible, what can this be owing to but a Consciousness of a Man's having done some thing Praise-worthy, and expressive of a great Soul? Whereas, if in all this he only Sacrificed to Vanity and Self-Love, as there would be nothing brave in Actions that make the most shining Appearance, so Nature would not have rewarded them with this divine Pleasure; nor could the Commendations, which a Person receives for Benefits done upon selfish Views, be at all more Satisfactory, than when he is applauded for what he doth without Design; because in both Cases the Ends of Self-Love are equally answered.
 The Conscience of approving ones self a Benefactor to Mankind is the noblest Recompence for being so; doubtless it is, and the most interested cannot propose anything so much to their own Advantage, notwithstanding which, the Inclination is nevertheless unselfish. The Pleasure which attends the Gratification of our Hunger and Thirst, is not the Cause of these Appetites; they are previous to any such Prospect; and so likewise is the DeSir e of doing Good; with this Difference, that being seated in the intellectual Part, this last, though Antecedent to Reason, may yet be improved and regulated by it, and, I will add, is no otherwise a Virtue than as it is so.
-Thus have I contended for the Dignity of that Nature I have the Honour to partake of, and, after all the Evidence produced, think I have a Right to conclude, against the Motto of this Paper, that there is such a thing as Generosity in the World. Though if I were under a Mistake in this, I should say as Cicero in Relation to the Immortality of the Soul, I willingly err, and should believe it very much for the Interest of Mankind to lye under the same Delusion. For the contrary Notion naturally tends to dispirit the Mind, and sinks it into a Meanness fatal to the Godlike Zeal of doing good. As on the other hand, it teaches People to be Ungrateful, by possessing them with a Perswasion concerning their Benefactors, that they have no Regard to them in the Benefits they bestow. Now he that banishes Gratitude from among Men, by so doing stops up the Stream of Beneficence. For though in conferring Kindnesses, a truly generous Man doth not aim at a Return, yet he looks to the Qualities of the Person obliged, and as nothing renders a Person more unworthy of a Benefit, than his being without all Resentment of it, he will not be extreamly forward to Oblige such a Man.
-</t>
+Thus have I contended for the Dignity of that Nature I have the Honour to partake of, and, after all the Evidence produced, think I have a Right to conclude, against the Motto of this Paper, that there is such a thing as Generosity in the World. Though if I were under a Mistake in this, I should say as Cicero in Relation to the Immortality of the Soul, I willingly err, and should believe it very much for the Interest of Mankind to lye under the same Delusion. For the contrary Notion naturally tends to dispirit the Mind, and sinks it into a Meanness fatal to the Godlike Zeal of doing good. As on the other hand, it teaches People to be Ungrateful, by possessing them with a Perswasion concerning their Benefactors, that they have no Regard to them in the Benefits they bestow. Now he that banishes Gratitude from among Men, by so doing stops up the Stream of Beneficence. For though in conferring Kindnesses, a truly generous Man doth not aim at a Return, yet he looks to the Qualities of the Person obliged, and as nothing renders a Person more unworthy of a Benefit, than his being without all Resentment of it, he will not be extreamly forward to Oblige such a Man.</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -1084,113 +1060,6 @@
         Bright Spears and shining Spear-men mount on high,</t>
   </si>
   <si>
-    <t xml:space="preserve">    'A large Collection of Manuscript Sermons preach'd by several of the most Eminent Divines, for some Years last past, are to be sold at the Bookseller's Warehouse in Exeter Change in the Strand.'
-    'This Day is publish'd,
-    'An Essay on Criticism. Printed for W. Lewis in Russell-street Covent Garden; and Sold by W. Taylor, at the Ship in Pater Noster Row; T. Osborn, in Grays-Inn near the Walks; J. Graves in St. James's-street; and J. Morphew near Stationers' Hall. Price 1s.'
-    'Concerning the Small-Pox.
-    'R. Stroughton, Apothecary, at the Unicorn in Southwark, having about Christmas last Published in the Postman, Tatler and Courant, a long Advertisement of his large Experience and great Success in curing the Small-Pox, even of the worst Kind and Circumstances, having had a Reputation for it almost 30 years, and can say than not 3 in 20 miscarry under his hands, doth now contract it; and only repeats, that he thinks he has attain'd to as great a Certainty therein (and the Measles which are near of Kin) as has been acquir'd in curing any one disease (an Intermitting Feaver with the Bark only excepted) which he conceives may at this time, when the Small-Pox so prevails, and is so mortal, justify his Publications, being pressed by several so to do, and hopes it may be for the Good of many: He has had many Patients since his last Publication and but One of all dy'd. He hath also Certificates from above 20 in a small time Cured, and of the worst sort. What is here offered is Truth and Matter of Fact; and he will, if desired, go with any one to the Persons themselves who have been Cured, many of whom are People of Value and Figure: 'Tis by a correct Management, more than a great deal of Physick, by which also the Face and Eyes are much secured; tho' one Secret he has (obtained only by Experience and which few or none know besides) that when they suddenly strike in very rarely fails of raising them again in a few Hours, when many other things, and proper too, have not answered. He does not desire, nor aim at the supplanting of any Physician or Apothecary concerned, but gives his assisting Advice if desired, and in such a way not Dishonourable or Injurious to either.'
-    'Angelick Snuff: The most noble Composition in the World, removing all manner of Disorders of the Head and all Swimming or Giddiness proceeding from Vapours, &amp;c., also Drowsiness, Sleepiness and other lethargick Effects, perfectly curing Deafness to Admiration, and ill Humours or Soreness in the Eyes, &amp;c., strength'ning them when weak, perfectly cures Catarrhs, or Defluxions of Rheum, and remedies the Tooth-ach instantly; is excellently beneficial in Apoplectick Fits and Falling-Sickness, and assuredly prevents those Distempers; corroborates the Brain, comforts the Nerves, and revives the Spirits. Its admirable Efficacy in all the above mention'd Diseases has been experienc'd above a Thousand times, and very justly causes it to be esteem'd the most beneficial Snuff in the World, being good for all sorts of Persons. Price 1s. a Paper with Directions. Sold only at Mr. Payn's Toyshop at the Angel and Crown in St Paul's Churchyard near Cheapside.'
-    'For Sale by the Candle,
-    'On Friday next, the 25th Instant, at Lloyd's Coffee-house in Lombard-Street at 4 a Clock in the Afternoon, only 1 Cask in a Lot, viz. 74 Buts, 22 Hogsheads and 3 quarter Casks of new Bene-Carlos Barcelona Wine, very deep, bright and strong, extraordinary good and ordinary, at £10. per. But, £5. per Hogshead and 25s. per Quarter Cask; neat, an entire Parcel, lately landed, now in Cellars on Galley Key (fronting the Thames) between the Coffeehouse and Tower Dock. To be tasted this Day the 23rd, and to Morrow the 24th Instant, from 7 a Clock to 1, and from 2 to 7, and all Friday till the Time of Sale. To be sold by Tho. Tomkins Broker in Seething-lane in Tower-street.'
-</t>
-  </si>
-  <si>
-    <t>But he who blends instruction with delight,
-Wins every reader, nor in vain shall write.
-(P.)
-180 	Hor.
-1 Ep. ii. 14. 	The monarch's folly makes the people rue.
-(P.)
-181 	Virg.
-Æn. ii. 145. 	Moved by these tears, we pity and protect.
-182 	Juv.
-Sat. vi. 180 	The bitter overbalances the sweet.
-183 	Hom. 	Sometimes fair truth in fiction we disguise;
-Sometimes present her naked to men's eyes.
-(Pope)
-184 	Hor.
-Ars Poet. v. 360. 	—Who labours long may be allowed sleep.
-185 	Virg.
-Æn. i. 15. 	And dwells such fury in celestial breasts?
-186 	Hor.
-3 Od. i. 38. 	High Heaven itself our impious rage assails.
-(P.)
-187 	Hor.</t>
-  </si>
-  <si>
-    <t>Sat. iii. 36 	With thumbs bent back, they popularly kill.
-(Dryden)
-437 	Ter.
-And. Act v. Sc. 4. 	Shall you escape with impunity; you who lay snares for young men of a liberal education, but unacquainted with the world, and by force of importunity and promises draw them in to marry harlots?
-438 	Hor.
-1 Ep. ii. 62. 	—Curb thy soul,
-And check thy rage, which must be ruled or rule.
-(Creech)
-439 	Ovid
-Metam. xii. 57 	Some tell what they have heard, or tales devise;
-Each fiction still improved with added lies.
-440 	Hor.
-2 Ep. ii. 213. 	Learn to live well, or fairly make your will.
-(Pope)
-441 	Hor.
-3 Od. iii. 7. 	Should the whole frame of nature round him break,
-In ruin and confusion hurl'd,
-He, unconcern'd, would hear the mighty crack,
-And stand secure amidst a falling world.
-(Anon.)
-442 	Hor.</t>
-  </si>
-  <si>
-    <t>241 	Virg.
-Æn. iv. 466. 	All sad she seems, forsaken, and alone;
-And left to wander wide through paths unknown.
-(P.)
-242 	Hor.
-2 Ep. i 168 	To write on vulgar themes, is thought an easy task.
-243 	Tull.
-Offic. 	You see, my son Marcus, virtue as if it were embodied, which if it could be made the object of sight, would (as Plato says) excite in us a wonderful love of wisdom.
-244 	Hor.
-2 Sat. vii. 101. 	A judge of painting you, a connoisseur.
-245 	Hor.
-Ars Poet. v. 338 	Fictions, to please, should wear the face of truth.
-246 		No amorous hero ever gave thee birth,
-Nor ever tender goddess brought thee forth:
-Some rugged rock's hard entrails gave thee form,
-And raging seas produced thee in a storm:
-A soul well suiting thy tempestuous kind,
-So rough thy manners, so untamed thy mind.
-(Pope)
-247 	Hesiod 	Their untired lips a wordy torrent pour.
-248 	Tull.
-Off. i. 16. 	It is a principal point of duty, to assist another most when he stands most in need of assistance.'
-249 	Frag. Vet. Poet. 	Mirth out of season is a grievous ill.
-250 	Hor.</t>
-  </si>
-  <si>
-    <t>(Creech)
-553 	Hor.
-1 Ep. xiv. 35. 	Once to be wild is no such foul disgrace,
-But 'tis so still to run the frantic race.
-(Creech)
-554 	Virg.
-Georg. iii. 9 	New ways I must attempt, my grovelling name
-To raise aloft, and wing my flight to fame.
-(Dryden)
-555 	Pers.
-Sat. iv. 51 	Lay the fictitious character aside.
-556 	Virg.
-Æn. ii. 471. 	So shines, renew'd in youth, the crested snake,
-Who slept the winter in a thorny brake;
-And, casting off his slough when spring returns,
-Now looks aloft, and with new glory burns:
-Restored with pois'nous herbs, his ardent sides
-Reflect the sun, and raised on spires he rides;
-High o'er the grass hissing he rolls along,
-And brandishes by fits his forky tongue.
-(Dryden)
-557 	Virg.</t>
-  </si>
-  <si>
     <t xml:space="preserve">As his father's eldest son, he had, on his return to England, family affairs to arrange, and probably some money to receive. Though attached to a party that lost power at the accession of Queen Anne, and waiting for new employment, Addison — who had declined the Duke of Somerset's over-condescending offer of a hundred a year and all expenses as travelling tutor to his son, the Marquis of Hertford — was able, while lodging poorly in the Haymarket, to associate in London with the men by whose friendship he hoped to rise, and was, with Steele, admitted into the select society of wits, and men of fashion who affected wit and took wits for their comrades, in the Kitcat Club. When in 1704 Marlborough's victory at Blenheim revived the Whig influence, the suggestion of Halifax to Lord Treasurer Godolphin caused Addison to be applied to for his poem of the Campaign. It was after the appearance of this poem that Steele's play was printed, with the dedication to his friend, in which he said,
     'I look upon my intimacy with you as one of the most valuable enjoyments of my life. At the same time I make the town no ill compliment for their kind acceptance of this comedy, in acknowledging that it has so far raised my opinion of it, as to make me think it no improper memorial of an inviolable Friendship. I should not offer it to you as such, had I not been very careful to avoid everything that might look ill-natured, immoral, or prejudicial to what the better part of mankind hold sacred and honourable.'
 This was the common ground between the friends. Collier's Short View of the Profaneness and Immorality of the English Stage had been published in 1698; it attacked a real evil, if not always in the right way, and Congreve's reply to it had been a failure. Steele's comedies with all their gaiety and humour were wholly free from the garnish of oaths and unwholesome expletives which his contemporaries seemed to think essential to stage emphasis. Each comedy of his was based on seriousness, as all sound English wit has been since there have been writers in England. The gay manner did not conceal all the earnest thoughts that might jar with the humour of the town; and thus Steele was able to claim, by right of his third play, 'the honour of being the only English dramatist who had had a piece damned for its piety.'
@@ -1409,9 +1278,6 @@
     <t>No. 617</t>
   </si>
   <si>
-    <t>No. 635</t>
-  </si>
-  <si>
     <t>Preface</t>
   </si>
   <si>
@@ -1560,9 +1426,6 @@
   </si>
   <si>
     <t>1714-11-08</t>
-  </si>
-  <si>
-    <t>1714-12-20</t>
   </si>
 </sst>
 </file>
@@ -1920,7 +1783,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1951,19 +1814,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
         <v>132</v>
       </c>
-      <c r="E2" t="s">
-        <v>138</v>
-      </c>
       <c r="F2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1971,19 +1834,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s">
         <v>133</v>
       </c>
-      <c r="E3" t="s">
-        <v>139</v>
-      </c>
       <c r="F3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1991,19 +1854,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F4" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2011,19 +1874,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2031,19 +1894,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F6" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2051,19 +1914,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F7" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2071,19 +1934,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F8" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2091,19 +1954,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F9" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2111,19 +1974,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F10" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2131,19 +1994,19 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2151,19 +2014,19 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2171,19 +2034,19 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2191,19 +2054,19 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E14" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F14" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2211,19 +2074,19 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F15" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2231,19 +2094,19 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F16" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2251,19 +2114,19 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E17" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F17" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2271,19 +2134,19 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E18" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F18" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2291,19 +2154,19 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F19" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2311,19 +2174,19 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E20" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F20" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2331,19 +2194,19 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E21" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F21" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2351,19 +2214,19 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F22" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2371,19 +2234,19 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E23" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F23" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2391,19 +2254,19 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E24" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F24" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2411,19 +2274,19 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E25" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F25" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2431,19 +2294,19 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E26" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2451,19 +2314,19 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F27" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2471,19 +2334,19 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E28" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F28" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2491,19 +2354,19 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E29" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F29" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2511,19 +2374,19 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E30" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F30" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2531,19 +2394,19 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E31" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F31" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2551,19 +2414,19 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F32" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2571,19 +2434,19 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E33" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F33" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2591,19 +2454,19 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E34" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F34" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2611,19 +2474,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E35" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F35" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2631,19 +2494,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E36" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F36" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2651,19 +2514,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E37" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F37" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2671,19 +2534,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F38" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2691,19 +2554,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E39" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F39" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2711,19 +2574,19 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E40" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F40" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2731,19 +2594,19 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E41" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F41" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2751,19 +2614,19 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E42" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F42" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2771,19 +2634,19 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F43" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2791,19 +2654,19 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E44" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F44" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2811,19 +2674,19 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E45" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F45" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2831,19 +2694,19 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E46" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F46" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2851,19 +2714,19 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D47" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E47" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F47" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2871,19 +2734,19 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D48" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E48" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F48" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2891,19 +2754,19 @@
         <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E49" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F49" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2911,19 +2774,19 @@
         <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E50" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F50" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2931,19 +2794,19 @@
         <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D51" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E51" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F51" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2951,19 +2814,19 @@
         <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E52" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F52" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2971,19 +2834,19 @@
         <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D53" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E53" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F53" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2991,19 +2854,19 @@
         <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D54" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E54" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F54" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3011,19 +2874,19 @@
         <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D55" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E55" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F55" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3031,19 +2894,19 @@
         <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D56" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E56" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F56" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3051,19 +2914,19 @@
         <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E57" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F57" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3071,19 +2934,19 @@
         <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D58" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E58" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F58" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3091,19 +2954,19 @@
         <v>49</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D59" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E59" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F59" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3111,19 +2974,19 @@
         <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D60" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E60" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F60" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3131,19 +2994,19 @@
         <v>50</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E61" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F61" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3151,19 +3014,19 @@
         <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D62" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E62" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F62" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -3171,19 +3034,19 @@
         <v>52</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D63" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E63" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F63" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3191,19 +3054,19 @@
         <v>53</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D64" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E64" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F64" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3211,19 +3074,19 @@
         <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D65" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E65" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F65" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3231,19 +3094,19 @@
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D66" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E66" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F66" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3251,19 +3114,19 @@
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D67" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E67" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F67" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3271,19 +3134,19 @@
         <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D68" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E68" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F68" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3291,119 +3154,19 @@
         <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C69" t="s">
+        <v>125</v>
+      </c>
+      <c r="D69" t="s">
         <v>126</v>
       </c>
-      <c r="D69" t="s">
-        <v>136</v>
-      </c>
       <c r="E69" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F69" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
-        <v>56</v>
-      </c>
-      <c r="B70" t="s">
-        <v>60</v>
-      </c>
-      <c r="C70" t="s">
-        <v>127</v>
-      </c>
-      <c r="D70" t="s">
-        <v>136</v>
-      </c>
-      <c r="E70" t="s">
-        <v>188</v>
-      </c>
-      <c r="F70" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" t="s">
-        <v>56</v>
-      </c>
-      <c r="B71" t="s">
-        <v>62</v>
-      </c>
-      <c r="C71" t="s">
-        <v>128</v>
-      </c>
-      <c r="D71" t="s">
-        <v>136</v>
-      </c>
-      <c r="E71" t="s">
-        <v>188</v>
-      </c>
-      <c r="F71" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" t="s">
-        <v>57</v>
-      </c>
-      <c r="B72" t="s">
-        <v>59</v>
-      </c>
-      <c r="C72" t="s">
-        <v>129</v>
-      </c>
-      <c r="D72" t="s">
-        <v>132</v>
-      </c>
-      <c r="E72" t="s">
-        <v>189</v>
-      </c>
-      <c r="F72" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" t="s">
-        <v>57</v>
-      </c>
-      <c r="B73" t="s">
-        <v>58</v>
-      </c>
-      <c r="C73" t="s">
-        <v>130</v>
-      </c>
-      <c r="D73" t="s">
-        <v>132</v>
-      </c>
-      <c r="E73" t="s">
-        <v>189</v>
-      </c>
-      <c r="F73" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" t="s">
-        <v>57</v>
-      </c>
-      <c r="B74" t="s">
-        <v>63</v>
-      </c>
-      <c r="C74" t="s">
-        <v>131</v>
-      </c>
-      <c r="D74" t="s">
-        <v>132</v>
-      </c>
-      <c r="E74" t="s">
-        <v>189</v>
-      </c>
-      <c r="F74" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>